<commit_message>
fixed percentile bug, added complete message
</commit_message>
<xml_diff>
--- a/recommended_trades.xlsx
+++ b/recommended_trades.xlsx
@@ -79,69 +79,69 @@
     <t>PYPL</t>
   </si>
   <si>
+    <t>LRCX</t>
+  </si>
+  <si>
     <t>IDXX</t>
   </si>
   <si>
-    <t>LRCX</t>
-  </si>
-  <si>
     <t>XLNX</t>
   </si>
   <si>
+    <t>DIS</t>
+  </si>
+  <si>
     <t>NTAP</t>
   </si>
   <si>
-    <t>DIS</t>
+    <t>TWTR</t>
   </si>
   <si>
     <t>QRVO</t>
   </si>
   <si>
+    <t>ZBRA</t>
+  </si>
+  <si>
+    <t>ALXN</t>
+  </si>
+  <si>
     <t>AES</t>
   </si>
   <si>
-    <t>TWTR</t>
-  </si>
-  <si>
-    <t>ZBRA</t>
-  </si>
-  <si>
-    <t>ALXN</t>
+    <t>IPGP</t>
   </si>
   <si>
     <t>AAPL</t>
   </si>
   <si>
+    <t>SNPS</t>
+  </si>
+  <si>
     <t>TTWO</t>
   </si>
   <si>
-    <t>SNPS</t>
-  </si>
-  <si>
-    <t>IPGP</t>
+    <t>DFS</t>
   </si>
   <si>
     <t>DVA</t>
   </si>
   <si>
-    <t>DFS</t>
-  </si>
-  <si>
     <t>PWR</t>
   </si>
   <si>
     <t>HCA</t>
   </si>
   <si>
+    <t>TPR</t>
+  </si>
+  <si>
     <t>AMD</t>
   </si>
   <si>
     <t>MU</t>
   </si>
   <si>
-    <t>TPR</t>
-  </si>
-  <si>
     <t>ADSK</t>
   </si>
   <si>
@@ -160,46 +160,46 @@
     <t>QCOM</t>
   </si>
   <si>
+    <t>MXIM</t>
+  </si>
+  <si>
     <t>SCHW</t>
   </si>
   <si>
     <t>FFIV</t>
   </si>
   <si>
-    <t>MXIM</t>
+    <t>PVH</t>
+  </si>
+  <si>
+    <t>DRI</t>
+  </si>
+  <si>
+    <t>ISRG</t>
+  </si>
+  <si>
+    <t>NLSN</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>IVZ</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>MGM</t>
   </si>
   <si>
     <t>AVGO</t>
   </si>
   <si>
-    <t>URI</t>
-  </si>
-  <si>
-    <t>NLSN</t>
-  </si>
-  <si>
-    <t>PVH</t>
-  </si>
-  <si>
-    <t>IVZ</t>
-  </si>
-  <si>
-    <t>DRI</t>
+    <t>KSS</t>
   </si>
   <si>
     <t>HWM</t>
-  </si>
-  <si>
-    <t>MGM</t>
-  </si>
-  <si>
-    <t>KSS</t>
-  </si>
-  <si>
-    <t>WY</t>
-  </si>
-  <si>
-    <t>ISRG</t>
   </si>
 </sst>
 </file>
@@ -630,37 +630,37 @@
         <v>12</v>
       </c>
       <c r="B2" s="2">
-        <v>25.01</v>
+        <v>25.11</v>
       </c>
       <c r="C2" s="2">
-        <v>0.9498728918651348</v>
+        <v>0.9590148168850288</v>
       </c>
       <c r="D2" s="3">
-        <v>98.81188118811882</v>
+        <v>0.9861386138613861</v>
       </c>
       <c r="E2" s="2">
-        <v>1.256257759410877</v>
+        <v>1.257790162022444</v>
       </c>
       <c r="F2" s="3">
-        <v>99.80198019801981</v>
+        <v>0.998019801980198</v>
       </c>
       <c r="G2" s="2">
-        <v>0.7126173229868998</v>
+        <v>0.7135333805389021</v>
       </c>
       <c r="H2" s="3">
-        <v>98.41584158415841</v>
+        <v>0.9841584158415841</v>
       </c>
       <c r="I2" s="2">
-        <v>0.1393031609428728</v>
+        <v>0.1410851731622056</v>
       </c>
       <c r="J2" s="3">
-        <v>91.88118811881188</v>
+        <v>0.9207920792079207</v>
       </c>
       <c r="K2" s="3">
-        <v>97.22772277227723</v>
+        <v>0.9722772277227723</v>
       </c>
       <c r="L2" s="4">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -668,37 +668,37 @@
         <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>151.73</v>
+        <v>149.87</v>
       </c>
       <c r="C3" s="2">
-        <v>1.112517687564886</v>
+        <v>1.152116884485056</v>
       </c>
       <c r="D3" s="3">
-        <v>99.20792079207921</v>
+        <v>0.9920792079207921</v>
       </c>
       <c r="E3" s="2">
-        <v>1.026196886022465</v>
+        <v>0.986450796182083</v>
       </c>
       <c r="F3" s="3">
-        <v>99.4059405940594</v>
+        <v>0.9900990099009901</v>
       </c>
       <c r="G3" s="2">
-        <v>0.8805201339585722</v>
+        <v>0.8725676497784354</v>
       </c>
       <c r="H3" s="3">
-        <v>99.60396039603961</v>
+        <v>0.9960396039603961</v>
       </c>
       <c r="I3" s="2">
-        <v>0.1252843745375631</v>
+        <v>0.1231872442734149</v>
       </c>
       <c r="J3" s="3">
-        <v>90.29702970297029</v>
+        <v>0.900990099009901</v>
       </c>
       <c r="K3" s="3">
-        <v>97.12871287128712</v>
+        <v>0.9698019801980198</v>
       </c>
       <c r="L3" s="4">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -706,34 +706,34 @@
         <v>14</v>
       </c>
       <c r="B4" s="2">
-        <v>534.12</v>
+        <v>537.24</v>
       </c>
       <c r="C4" s="2">
-        <v>0.8940348263442406</v>
+        <v>0.9162690348752154</v>
       </c>
       <c r="D4" s="3">
-        <v>98.01980198019803</v>
+        <v>0.9821782178217822</v>
       </c>
       <c r="E4" s="2">
-        <v>1.000879190015052</v>
+        <v>1.004801626597651</v>
       </c>
       <c r="F4" s="3">
-        <v>99.20792079207921</v>
+        <v>0.9920792079207921</v>
       </c>
       <c r="G4" s="2">
-        <v>0.705682113190104</v>
+        <v>0.7288398237355709</v>
       </c>
       <c r="H4" s="3">
-        <v>97.82178217821782</v>
+        <v>0.9861386138613861</v>
       </c>
       <c r="I4" s="2">
-        <v>0.1060955236564328</v>
+        <v>0.1034375529710665</v>
       </c>
       <c r="J4" s="3">
-        <v>87.52475247524752</v>
+        <v>0.8613861386138614</v>
       </c>
       <c r="K4" s="3">
-        <v>95.64356435643565</v>
+        <v>0.9554455445544554</v>
       </c>
       <c r="L4" s="4">
         <v>37</v>
@@ -744,37 +744,37 @@
         <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>463.77</v>
+        <v>477.62</v>
       </c>
       <c r="C5" s="2">
-        <v>0.7874199566541374</v>
+        <v>0.786943399714908</v>
       </c>
       <c r="D5" s="3">
-        <v>96.63366336633663</v>
+        <v>0.9643564356435644</v>
       </c>
       <c r="E5" s="2">
-        <v>0.4206618785195841</v>
+        <v>0.4146027699208799</v>
       </c>
       <c r="F5" s="3">
-        <v>83.76237623762377</v>
+        <v>0.8316831683168318</v>
       </c>
       <c r="G5" s="2">
-        <v>0.7127280395186162</v>
+        <v>0.6874853912370475</v>
       </c>
       <c r="H5" s="3">
-        <v>98.61386138613861</v>
+        <v>0.9762376237623762</v>
       </c>
       <c r="I5" s="2">
-        <v>0.160289481600644</v>
+        <v>0.1579186773318177</v>
       </c>
       <c r="J5" s="3">
-        <v>94.65346534653466</v>
+        <v>0.9485148514851486</v>
       </c>
       <c r="K5" s="3">
-        <v>93.41584158415841</v>
+        <v>0.9301980198019802</v>
       </c>
       <c r="L5" s="4">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -782,34 +782,34 @@
         <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>380.88</v>
+        <v>378.43</v>
       </c>
       <c r="C6" s="2">
-        <v>0.5004713935003846</v>
+        <v>0.5176504066216219</v>
       </c>
       <c r="D6" s="3">
-        <v>91.88118811881188</v>
+        <v>0.9227722772277228</v>
       </c>
       <c r="E6" s="2">
-        <v>0.7452858422905101</v>
+        <v>0.7351015215157077</v>
       </c>
       <c r="F6" s="3">
-        <v>97.22772277227723</v>
+        <v>0.9702970297029703</v>
       </c>
       <c r="G6" s="2">
-        <v>0.6719789393336744</v>
+        <v>0.6712749581550093</v>
       </c>
       <c r="H6" s="3">
-        <v>97.22772277227723</v>
+        <v>0.9742574257425742</v>
       </c>
       <c r="I6" s="2">
-        <v>0.08300484271877089</v>
+        <v>0.0839015744672628</v>
       </c>
       <c r="J6" s="3">
-        <v>80</v>
+        <v>0.807920792079208</v>
       </c>
       <c r="K6" s="3">
-        <v>91.58415841584159</v>
+        <v>0.9188118811881189</v>
       </c>
       <c r="L6" s="4">
         <v>52</v>
@@ -820,37 +820,37 @@
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C7" s="2">
-        <v>0.9192916741321954</v>
+        <v>0.9376139846032736</v>
       </c>
       <c r="D7" s="3">
-        <v>98.41584158415841</v>
+        <v>0.9841584158415841</v>
       </c>
       <c r="E7" s="2">
-        <v>0.4178659275391022</v>
+        <v>0.4245207159450878</v>
       </c>
       <c r="F7" s="3">
-        <v>83.36633663366337</v>
+        <v>0.8495049504950495</v>
       </c>
       <c r="G7" s="2">
-        <v>0.3457082572433398</v>
+        <v>0.3488279878125092</v>
       </c>
       <c r="H7" s="3">
-        <v>79.20792079207921</v>
+        <v>0.7960396039603961</v>
       </c>
       <c r="I7" s="2">
-        <v>0.2001724158950683</v>
+        <v>0.2055347874666858</v>
       </c>
       <c r="J7" s="3">
-        <v>97.82178217821782</v>
+        <v>0.9801980198019803</v>
       </c>
       <c r="K7" s="3">
-        <v>89.70297029702971</v>
+        <v>0.9024752475247525</v>
       </c>
       <c r="L7" s="4">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -858,37 +858,37 @@
         <v>18</v>
       </c>
       <c r="B8" s="2">
-        <v>134.69</v>
+        <v>129.32</v>
       </c>
       <c r="C8" s="2">
-        <v>0.3509126513653863</v>
+        <v>0.3529197131681786</v>
       </c>
       <c r="D8" s="3">
-        <v>82.57425742574257</v>
+        <v>0.8257425742574257</v>
       </c>
       <c r="E8" s="2">
-        <v>0.6523469562899753</v>
+        <v>0.6464635492290159</v>
       </c>
       <c r="F8" s="3">
-        <v>95.24752475247524</v>
+        <v>0.9504950495049505</v>
       </c>
       <c r="G8" s="2">
-        <v>0.5310272037111515</v>
+        <v>0.5453197537965351</v>
       </c>
       <c r="H8" s="3">
-        <v>94.65346534653466</v>
+        <v>0.9485148514851486</v>
       </c>
       <c r="I8" s="2">
-        <v>0.1008191007363557</v>
+        <v>0.1035294765061404</v>
       </c>
       <c r="J8" s="3">
-        <v>85.74257425742574</v>
+        <v>0.8633663366336635</v>
       </c>
       <c r="K8" s="3">
-        <v>89.55445544554456</v>
+        <v>0.897029702970297</v>
       </c>
       <c r="L8" s="4">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -896,37 +896,37 @@
         <v>19</v>
       </c>
       <c r="B9" s="2">
-        <v>70.52</v>
+        <v>68.77</v>
       </c>
       <c r="C9" s="2">
-        <v>0.3944986234532237</v>
+        <v>0.3987128111649818</v>
       </c>
       <c r="D9" s="3">
-        <v>85.54455445544555</v>
+        <v>0.8534653465346534</v>
       </c>
       <c r="E9" s="2">
-        <v>0.4491069622613672</v>
+        <v>0.461145477678692</v>
       </c>
       <c r="F9" s="3">
-        <v>85.94059405940594</v>
+        <v>0.8712871287128714</v>
       </c>
       <c r="G9" s="2">
-        <v>0.5017407443288395</v>
+        <v>0.4916545463603517</v>
       </c>
       <c r="H9" s="3">
-        <v>93.26732673267327</v>
+        <v>0.9247524752475248</v>
       </c>
       <c r="I9" s="2">
-        <v>0.13207619502356</v>
+        <v>0.13391624128575</v>
       </c>
       <c r="J9" s="3">
-        <v>91.28712871287129</v>
+        <v>0.9148514851485149</v>
       </c>
       <c r="K9" s="3">
-        <v>89.00990099009901</v>
+        <v>0.8910891089108911</v>
       </c>
       <c r="L9" s="4">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -934,37 +934,37 @@
         <v>20</v>
       </c>
       <c r="B10" s="2">
-        <v>242.05</v>
+        <v>249.93</v>
       </c>
       <c r="C10" s="2">
-        <v>1.232735901987945</v>
+        <v>1.245702530411826</v>
       </c>
       <c r="D10" s="3">
-        <v>99.80198019801981</v>
+        <v>0.998019801980198</v>
       </c>
       <c r="E10" s="2">
-        <v>0.3998477200241078</v>
+        <v>0.3933687179648661</v>
       </c>
       <c r="F10" s="3">
-        <v>80.5940594059406</v>
+        <v>0.7980198019801981</v>
       </c>
       <c r="G10" s="2">
-        <v>0.3273007290213317</v>
+        <v>0.3239523293603485</v>
       </c>
       <c r="H10" s="3">
-        <v>75.84158415841584</v>
+        <v>0.7584158415841584</v>
       </c>
       <c r="I10" s="2">
-        <v>0.2006762818807902</v>
+        <v>0.1996891795640673</v>
       </c>
       <c r="J10" s="3">
-        <v>98.01980198019803</v>
+        <v>0.9782178217821782</v>
       </c>
       <c r="K10" s="3">
-        <v>88.56435643564356</v>
+        <v>0.8831683168316832</v>
       </c>
       <c r="L10" s="4">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -972,34 +972,34 @@
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>498.59</v>
+        <v>492.51</v>
       </c>
       <c r="C11" s="2">
-        <v>0.881898182781264</v>
+        <v>0.642729926752745</v>
       </c>
       <c r="D11" s="3">
-        <v>97.62376237623762</v>
+        <v>0.9445544554455445</v>
       </c>
       <c r="E11" s="2">
-        <v>0.5135233899008885</v>
+        <v>0.5136562507030719</v>
       </c>
       <c r="F11" s="3">
-        <v>91.88118811881188</v>
+        <v>0.9188118811881187</v>
       </c>
       <c r="G11" s="2">
-        <v>0.3738659949777831</v>
+        <v>0.5023244104072498</v>
       </c>
       <c r="H11" s="3">
-        <v>82.77227722772277</v>
+        <v>0.9326732673267327</v>
       </c>
       <c r="I11" s="2">
-        <v>0.0745176537294413</v>
+        <v>0.05473792071197206</v>
       </c>
       <c r="J11" s="3">
-        <v>76.63366336633663</v>
+        <v>0.693069306930693</v>
       </c>
       <c r="K11" s="3">
-        <v>87.22772277227722</v>
+        <v>0.8722772277227723</v>
       </c>
       <c r="L11" s="4">
         <v>40</v>
@@ -1010,37 +1010,37 @@
         <v>22</v>
       </c>
       <c r="B12" s="2">
-        <v>502.8</v>
+        <v>518.2</v>
       </c>
       <c r="C12" s="2">
-        <v>0.638989376072399</v>
+        <v>0.907047151285176</v>
       </c>
       <c r="D12" s="3">
-        <v>94.25742574257426</v>
+        <v>0.9801980198019803</v>
       </c>
       <c r="E12" s="2">
-        <v>0.5097834120875135</v>
+        <v>0.507643548541111</v>
       </c>
       <c r="F12" s="3">
-        <v>91.48514851485149</v>
+        <v>0.9128712871287129</v>
       </c>
       <c r="G12" s="2">
-        <v>0.5051698992014361</v>
+        <v>0.3649684388110375</v>
       </c>
       <c r="H12" s="3">
-        <v>93.66336633663366</v>
+        <v>0.8158415841584159</v>
       </c>
       <c r="I12" s="2">
-        <v>0.05360336250814954</v>
+        <v>0.07416185373068887</v>
       </c>
       <c r="J12" s="3">
-        <v>68.91089108910892</v>
+        <v>0.7663366336633664</v>
       </c>
       <c r="K12" s="3">
-        <v>87.07920792079207</v>
+        <v>0.8688118811881189</v>
       </c>
       <c r="L12" s="4">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1048,37 +1048,37 @@
         <v>23</v>
       </c>
       <c r="B13" s="2">
-        <v>146.34</v>
+        <v>147.52</v>
       </c>
       <c r="C13" s="2">
-        <v>0.4668529145780964</v>
+        <v>0.4794050877131514</v>
       </c>
       <c r="D13" s="3">
-        <v>91.28712871287129</v>
+        <v>0.9168316831683169</v>
       </c>
       <c r="E13" s="2">
-        <v>0.5004772480367677</v>
+        <v>0.5084114149480617</v>
       </c>
       <c r="F13" s="3">
-        <v>90.89108910891089</v>
+        <v>0.9148514851485149</v>
       </c>
       <c r="G13" s="2">
-        <v>0.475057881028231</v>
+        <v>0.4648226492943011</v>
       </c>
       <c r="H13" s="3">
-        <v>91.88118811881188</v>
+        <v>0.9108910891089108</v>
       </c>
       <c r="I13" s="2">
-        <v>0.06653654146009774</v>
+        <v>0.06656368081518971</v>
       </c>
       <c r="J13" s="3">
-        <v>73.46534653465346</v>
+        <v>0.7306930693069308</v>
       </c>
       <c r="K13" s="3">
-        <v>86.88118811881188</v>
+        <v>0.8683168316831683</v>
       </c>
       <c r="L13" s="4">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1086,37 +1086,37 @@
         <v>24</v>
       </c>
       <c r="B14" s="2">
-        <v>68.90000000000001</v>
+        <v>175.73</v>
       </c>
       <c r="C14" s="2">
-        <v>0.1017136715995174</v>
+        <v>0.204354004088294</v>
       </c>
       <c r="D14" s="3">
-        <v>53.86138613861386</v>
+        <v>0.6811881188118812</v>
       </c>
       <c r="E14" s="2">
-        <v>0.6229775186297619</v>
+        <v>0.4898951461879383</v>
       </c>
       <c r="F14" s="3">
-        <v>94.65346534653466</v>
+        <v>0.9029702970297029</v>
       </c>
       <c r="G14" s="2">
-        <v>0.6470205113476261</v>
+        <v>0.4236745655979644</v>
       </c>
       <c r="H14" s="3">
-        <v>96.43564356435644</v>
+        <v>0.887128712871287</v>
       </c>
       <c r="I14" s="2">
-        <v>0.2399816595293026</v>
+        <v>0.1899863174686581</v>
       </c>
       <c r="J14" s="3">
-        <v>99.20792079207921</v>
+        <v>0.9742574257425742</v>
       </c>
       <c r="K14" s="3">
-        <v>86.03960396039604</v>
+        <v>0.8613861386138614</v>
       </c>
       <c r="L14" s="4">
-        <v>290</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1124,37 +1124,37 @@
         <v>25</v>
       </c>
       <c r="B15" s="2">
-        <v>182.4</v>
+        <v>67.7</v>
       </c>
       <c r="C15" s="2">
-        <v>0.2043764742370394</v>
+        <v>0.09993295864676441</v>
       </c>
       <c r="D15" s="3">
-        <v>68.11881188118812</v>
+        <v>0.5386138613861386</v>
       </c>
       <c r="E15" s="2">
-        <v>0.4924128673947684</v>
+        <v>0.6149190818271457</v>
       </c>
       <c r="F15" s="3">
-        <v>90.29702970297029</v>
+        <v>0.9465346534653466</v>
       </c>
       <c r="G15" s="2">
-        <v>0.4142635268775257</v>
+        <v>0.6489598983406454</v>
       </c>
       <c r="H15" s="3">
-        <v>88.11881188118812</v>
+        <v>0.9663366336633663</v>
       </c>
       <c r="I15" s="2">
-        <v>0.1928751870054605</v>
+        <v>0.2355986101987756</v>
       </c>
       <c r="J15" s="3">
-        <v>97.42574257425743</v>
+        <v>0.9920792079207921</v>
       </c>
       <c r="K15" s="3">
-        <v>85.99009900990099</v>
+        <v>0.8608910891089109</v>
       </c>
       <c r="L15" s="4">
-        <v>109</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1162,37 +1162,37 @@
         <v>26</v>
       </c>
       <c r="B16" s="2">
-        <v>173.31</v>
+        <v>55.32</v>
       </c>
       <c r="C16" s="2">
-        <v>0.430116258859344</v>
+        <v>0.6918159072706545</v>
       </c>
       <c r="D16" s="3">
-        <v>88.51485148514851</v>
+        <v>0.9544554455445545</v>
       </c>
       <c r="E16" s="2">
-        <v>0.4932130345712405</v>
+        <v>0.673505449470471</v>
       </c>
       <c r="F16" s="3">
-        <v>90.4950495049505</v>
+        <v>0.9564356435643565</v>
       </c>
       <c r="G16" s="2">
-        <v>0.3236468027203759</v>
+        <v>0.2040038095009978</v>
       </c>
       <c r="H16" s="3">
-        <v>75.04950495049505</v>
+        <v>0.5227722772277228</v>
       </c>
       <c r="I16" s="2">
-        <v>0.1079024301450009</v>
+        <v>0.2165900295314206</v>
       </c>
       <c r="J16" s="3">
-        <v>88.11881188118812</v>
+        <v>0.9861386138613861</v>
       </c>
       <c r="K16" s="3">
-        <v>85.54455445544555</v>
+        <v>0.854950495049505</v>
       </c>
       <c r="L16" s="4">
-        <v>115</v>
+        <v>361</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1200,37 +1200,37 @@
         <v>27</v>
       </c>
       <c r="B17" s="2">
-        <v>24.21</v>
+        <v>173.19</v>
       </c>
       <c r="C17" s="2">
-        <v>0.2344727395869677</v>
+        <v>0.4233556200031775</v>
       </c>
       <c r="D17" s="3">
-        <v>71.68316831683168</v>
+        <v>0.8831683168316832</v>
       </c>
       <c r="E17" s="2">
-        <v>0.748291502739745</v>
+        <v>0.4755393904144772</v>
       </c>
       <c r="F17" s="3">
-        <v>97.42574257425743</v>
+        <v>0.8891089108910891</v>
       </c>
       <c r="G17" s="2">
-        <v>0.3474998429756647</v>
+        <v>0.3228041076835305</v>
       </c>
       <c r="H17" s="3">
-        <v>79.60396039603961</v>
+        <v>0.7524752475247525</v>
       </c>
       <c r="I17" s="2">
-        <v>0.1518084325770427</v>
+        <v>0.1116579477301163</v>
       </c>
       <c r="J17" s="3">
-        <v>93.46534653465346</v>
+        <v>0.8811881188118812</v>
       </c>
       <c r="K17" s="3">
-        <v>85.54455445544555</v>
+        <v>0.8514851485148515</v>
       </c>
       <c r="L17" s="4">
-        <v>826</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1238,37 +1238,37 @@
         <v>28</v>
       </c>
       <c r="B18" s="2">
-        <v>55.6</v>
+        <v>386.41</v>
       </c>
       <c r="C18" s="2">
-        <v>0.6799029832924814</v>
+        <v>0.488604042926585</v>
       </c>
       <c r="D18" s="3">
-        <v>95.24752475247524</v>
+        <v>0.9188118811881187</v>
       </c>
       <c r="E18" s="2">
-        <v>0.665299620469158</v>
+        <v>0.465501022530267</v>
       </c>
       <c r="F18" s="3">
-        <v>95.64356435643565</v>
+        <v>0.8752475247524752</v>
       </c>
       <c r="G18" s="2">
-        <v>0.2071103789997448</v>
+        <v>0.5326782909712451</v>
       </c>
       <c r="H18" s="3">
-        <v>52.87128712871287</v>
+        <v>0.9465346534653466</v>
       </c>
       <c r="I18" s="2">
-        <v>0.2085399071265994</v>
+        <v>0.04853467059964991</v>
       </c>
       <c r="J18" s="3">
-        <v>98.21782178217822</v>
+        <v>0.6633663366336634</v>
       </c>
       <c r="K18" s="3">
-        <v>85.4950495049505</v>
+        <v>0.850990099009901</v>
       </c>
       <c r="L18" s="4">
-        <v>359</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1276,37 +1276,37 @@
         <v>29</v>
       </c>
       <c r="B19" s="2">
-        <v>385.71</v>
+        <v>152.93</v>
       </c>
       <c r="C19" s="2">
-        <v>0.502756219441796</v>
+        <v>0.3998837031084408</v>
       </c>
       <c r="D19" s="3">
-        <v>92.07920792079207</v>
+        <v>0.8594059405940594</v>
       </c>
       <c r="E19" s="2">
-        <v>0.46835285699715</v>
+        <v>0.3404332744348608</v>
       </c>
       <c r="F19" s="3">
-        <v>88.31683168316832</v>
+        <v>0.7306930693069308</v>
       </c>
       <c r="G19" s="2">
-        <v>0.5357445398595293</v>
+        <v>0.3631388445934839</v>
       </c>
       <c r="H19" s="3">
-        <v>94.85148514851485</v>
+        <v>0.8118811881188118</v>
       </c>
       <c r="I19" s="2">
-        <v>0.04814341230455092</v>
+        <v>0.2606243365559723</v>
       </c>
       <c r="J19" s="3">
-        <v>65.94059405940594</v>
+        <v>0.9960396039603961</v>
       </c>
       <c r="K19" s="3">
-        <v>85.29702970297029</v>
+        <v>0.8495049504950496</v>
       </c>
       <c r="L19" s="4">
-        <v>51</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1314,37 +1314,37 @@
         <v>30</v>
       </c>
       <c r="B20" s="2">
-        <v>157.95</v>
+        <v>24.37</v>
       </c>
       <c r="C20" s="2">
-        <v>0.3987930221708954</v>
+        <v>0.2300965002083619</v>
       </c>
       <c r="D20" s="3">
-        <v>86.53465346534654</v>
+        <v>0.7089108910891089</v>
       </c>
       <c r="E20" s="2">
-        <v>0.3290787987718349</v>
+        <v>0.739717602459051</v>
       </c>
       <c r="F20" s="3">
-        <v>71.68316831683168</v>
+        <v>0.9722772277227724</v>
       </c>
       <c r="G20" s="2">
-        <v>0.3649080144980603</v>
+        <v>0.3407771916841148</v>
       </c>
       <c r="H20" s="3">
-        <v>81.98019801980197</v>
+        <v>0.7821782178217822</v>
       </c>
       <c r="I20" s="2">
-        <v>0.2582216300932443</v>
+        <v>0.150262784868845</v>
       </c>
       <c r="J20" s="3">
-        <v>99.60396039603961</v>
+        <v>0.9326732673267327</v>
       </c>
       <c r="K20" s="3">
-        <v>84.95049504950495</v>
+        <v>0.8490099009900991</v>
       </c>
       <c r="L20" s="4">
-        <v>126</v>
+        <v>820</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1352,37 +1352,37 @@
         <v>31</v>
       </c>
       <c r="B21" s="2">
-        <v>134.61</v>
+        <v>227.7</v>
       </c>
       <c r="C21" s="2">
-        <v>0.8925169458712732</v>
+        <v>0.5269899941530005</v>
       </c>
       <c r="D21" s="3">
-        <v>97.82178217821782</v>
+        <v>0.9267326732673267</v>
       </c>
       <c r="E21" s="2">
-        <v>0.4552349252657163</v>
+        <v>0.3803364274844884</v>
       </c>
       <c r="F21" s="3">
-        <v>86.53465346534654</v>
+        <v>0.7801980198019802</v>
       </c>
       <c r="G21" s="2">
-        <v>0.2349838412770883</v>
+        <v>0.38928163489564</v>
       </c>
       <c r="H21" s="3">
-        <v>59.80198019801981</v>
+        <v>0.8554455445544555</v>
       </c>
       <c r="I21" s="2">
-        <v>0.156021039410469</v>
+        <v>0.08548102803219773</v>
       </c>
       <c r="J21" s="3">
-        <v>94.25742574257426</v>
+        <v>0.8118811881188118</v>
       </c>
       <c r="K21" s="3">
-        <v>84.60396039603961</v>
+        <v>0.8435643564356435</v>
       </c>
       <c r="L21" s="4">
-        <v>148</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1390,37 +1390,37 @@
         <v>32</v>
       </c>
       <c r="B22" s="2">
-        <v>208.6</v>
+        <v>137.48</v>
       </c>
       <c r="C22" s="2">
-        <v>0.677208029254834</v>
+        <v>0.8892862785584729</v>
       </c>
       <c r="D22" s="3">
-        <v>95.04950495049505</v>
+        <v>0.9762376237623762</v>
       </c>
       <c r="E22" s="2">
-        <v>0.4225117769478845</v>
+        <v>0.4448359404215095</v>
       </c>
       <c r="F22" s="3">
-        <v>84.15841584158416</v>
+        <v>0.8574257425742574</v>
       </c>
       <c r="G22" s="2">
-        <v>0.2446040486449453</v>
+        <v>0.2275474803786745</v>
       </c>
       <c r="H22" s="3">
-        <v>61.78217821782178</v>
+        <v>0.5861386138613862</v>
       </c>
       <c r="I22" s="2">
-        <v>0.1797500484540301</v>
+        <v>0.1549563461945225</v>
       </c>
       <c r="J22" s="3">
-        <v>96.83168316831683</v>
+        <v>0.9405940594059407</v>
       </c>
       <c r="K22" s="3">
-        <v>84.45544554455445</v>
+        <v>0.8400990099009902</v>
       </c>
       <c r="L22" s="4">
-        <v>95</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1428,37 +1428,37 @@
         <v>33</v>
       </c>
       <c r="B23" s="2">
-        <v>264.09</v>
+        <v>257.29</v>
       </c>
       <c r="C23" s="2">
-        <v>0.8504912745415401</v>
+        <v>0.85610341687993</v>
       </c>
       <c r="D23" s="3">
-        <v>97.42574257425743</v>
+        <v>0.9742574257425742</v>
       </c>
       <c r="E23" s="2">
-        <v>0.3351626493924595</v>
+        <v>0.3269862625421225</v>
       </c>
       <c r="F23" s="3">
-        <v>72.27722772277228</v>
+        <v>0.7108910891089109</v>
       </c>
       <c r="G23" s="2">
-        <v>0.2900956623325551</v>
+        <v>0.2873255288449595</v>
       </c>
       <c r="H23" s="3">
-        <v>70.6930693069307</v>
+        <v>0.7029702970297029</v>
       </c>
       <c r="I23" s="2">
-        <v>0.1839822028323888</v>
+        <v>0.1857506614605424</v>
       </c>
       <c r="J23" s="3">
-        <v>97.02970297029702</v>
+        <v>0.9702970297029703</v>
       </c>
       <c r="K23" s="3">
-        <v>84.35643564356435</v>
+        <v>0.8396039603960396</v>
       </c>
       <c r="L23" s="4">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1466,37 +1466,37 @@
         <v>34</v>
       </c>
       <c r="B24" s="2">
-        <v>228.18</v>
+        <v>210.4</v>
       </c>
       <c r="C24" s="2">
-        <v>0.5317792182411814</v>
+        <v>0.683403193320515</v>
       </c>
       <c r="D24" s="3">
-        <v>92.67326732673267</v>
+        <v>0.9504950495049505</v>
       </c>
       <c r="E24" s="2">
-        <v>0.379823970063865</v>
+        <v>0.408950322924624</v>
       </c>
       <c r="F24" s="3">
-        <v>78.01980198019803</v>
+        <v>0.8178217821782178</v>
       </c>
       <c r="G24" s="2">
-        <v>0.3908402298471535</v>
+        <v>0.2479348343273408</v>
       </c>
       <c r="H24" s="3">
-        <v>84.75247524752476</v>
+        <v>0.6237623762376238</v>
       </c>
       <c r="I24" s="2">
-        <v>0.08572713156406653</v>
+        <v>0.1793054004107653</v>
       </c>
       <c r="J24" s="3">
-        <v>81.18811881188118</v>
+        <v>0.9643564356435644</v>
       </c>
       <c r="K24" s="3">
-        <v>84.15841584158416</v>
+        <v>0.8391089108910891</v>
       </c>
       <c r="L24" s="4">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1504,37 +1504,37 @@
         <v>35</v>
       </c>
       <c r="B25" s="2">
-        <v>115.82</v>
+        <v>92.15000000000001</v>
       </c>
       <c r="C25" s="2">
-        <v>0.5671339856107744</v>
+        <v>0.06969134149192137</v>
       </c>
       <c r="D25" s="3">
-        <v>93.46534653465346</v>
+        <v>0.497029702970297</v>
       </c>
       <c r="E25" s="2">
-        <v>0.474367149250828</v>
+        <v>0.6576050503872044</v>
       </c>
       <c r="F25" s="3">
-        <v>88.91089108910892</v>
+        <v>0.9544554455445545</v>
       </c>
       <c r="G25" s="2">
-        <v>0.4126222697028553</v>
+        <v>0.695160487811968</v>
       </c>
       <c r="H25" s="3">
-        <v>87.72277227722772</v>
+        <v>0.9801980198019803</v>
       </c>
       <c r="I25" s="2">
-        <v>0.0464937283509325</v>
+        <v>0.1312915349255158</v>
       </c>
       <c r="J25" s="3">
-        <v>64.55445544554455</v>
+        <v>0.9108910891089108</v>
       </c>
       <c r="K25" s="3">
-        <v>83.66336633663366</v>
+        <v>0.8356435643564357</v>
       </c>
       <c r="L25" s="4">
-        <v>172</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1542,37 +1542,37 @@
         <v>36</v>
       </c>
       <c r="B26" s="2">
-        <v>90.28</v>
+        <v>117.27</v>
       </c>
       <c r="C26" s="2">
-        <v>0.07051491251711976</v>
+        <v>0.5683466434238769</v>
       </c>
       <c r="D26" s="3">
-        <v>49.7029702970297</v>
+        <v>0.9346534653465346</v>
       </c>
       <c r="E26" s="2">
-        <v>0.6420891701178916</v>
+        <v>0.461678644908458</v>
       </c>
       <c r="F26" s="3">
-        <v>94.85148514851485</v>
+        <v>0.8732673267326733</v>
       </c>
       <c r="G26" s="2">
-        <v>0.699837083407752</v>
+        <v>0.409508140739746</v>
       </c>
       <c r="H26" s="3">
-        <v>97.62376237623762</v>
+        <v>0.8732673267326733</v>
       </c>
       <c r="I26" s="2">
-        <v>0.1319224183149583</v>
+        <v>0.0466719526532492</v>
       </c>
       <c r="J26" s="3">
-        <v>91.08910891089108</v>
+        <v>0.6475247524752475</v>
       </c>
       <c r="K26" s="3">
-        <v>83.31683168316832</v>
+        <v>0.8321782178217821</v>
       </c>
       <c r="L26" s="4">
-        <v>221</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1580,34 +1580,34 @@
         <v>37</v>
       </c>
       <c r="B27" s="2">
-        <v>72.42</v>
+        <v>72.23</v>
       </c>
       <c r="C27" s="2">
-        <v>0.755799333560764</v>
+        <v>0.728264327216755</v>
       </c>
       <c r="D27" s="3">
-        <v>96.03960396039604</v>
+        <v>0.9603960396039604</v>
       </c>
       <c r="E27" s="2">
-        <v>0.8126395945353205</v>
+        <v>0.8160518492417379</v>
       </c>
       <c r="F27" s="3">
-        <v>98.21782178217822</v>
+        <v>0.9801980198019803</v>
       </c>
       <c r="G27" s="2">
-        <v>0.3888903650630721</v>
+        <v>0.3842377808353003</v>
       </c>
       <c r="H27" s="3">
-        <v>84.35643564356435</v>
+        <v>0.8455445544554455</v>
       </c>
       <c r="I27" s="2">
-        <v>0.02774462555368226</v>
+        <v>0.02880716649867547</v>
       </c>
       <c r="J27" s="3">
-        <v>53.06930693069307</v>
+        <v>0.5366336633663367</v>
       </c>
       <c r="K27" s="3">
-        <v>82.92079207920791</v>
+        <v>0.8306930693069308</v>
       </c>
       <c r="L27" s="4">
         <v>276</v>
@@ -1618,37 +1618,37 @@
         <v>38</v>
       </c>
       <c r="B28" s="2">
-        <v>171.8</v>
+        <v>164.39</v>
       </c>
       <c r="C28" s="2">
-        <v>0.1243554941386676</v>
+        <v>0.1227878162079462</v>
       </c>
       <c r="D28" s="3">
-        <v>58.01980198019802</v>
+        <v>0.5801980198019802</v>
       </c>
       <c r="E28" s="2">
-        <v>0.679174950439173</v>
+        <v>0.7039964410953991</v>
       </c>
       <c r="F28" s="3">
-        <v>95.84158415841584</v>
+        <v>0.9623762376237623</v>
       </c>
       <c r="G28" s="2">
-        <v>0.4422257881935131</v>
+        <v>0.4276379037410283</v>
       </c>
       <c r="H28" s="3">
-        <v>89.5049504950495</v>
+        <v>0.8910891089108911</v>
       </c>
       <c r="I28" s="2">
-        <v>0.1103104406335618</v>
+        <v>0.114082502971648</v>
       </c>
       <c r="J28" s="3">
-        <v>88.31683168316832</v>
+        <v>0.8891089108910891</v>
       </c>
       <c r="K28" s="3">
-        <v>82.92079207920791</v>
+        <v>0.8306930693069307</v>
       </c>
       <c r="L28" s="4">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1656,37 +1656,37 @@
         <v>39</v>
       </c>
       <c r="B29" s="2">
-        <v>91.94</v>
+        <v>31.87</v>
       </c>
       <c r="C29" s="2">
-        <v>1.063884796538701</v>
+        <v>0.1489780454771879</v>
       </c>
       <c r="D29" s="3">
-        <v>99.00990099009901</v>
+        <v>0.6079207920792079</v>
       </c>
       <c r="E29" s="2">
-        <v>0.6978714429136357</v>
+        <v>1.230555426375541</v>
       </c>
       <c r="F29" s="3">
-        <v>96.43564356435644</v>
+        <v>0.9960396039603961</v>
       </c>
       <c r="G29" s="2">
-        <v>0.2266482714218559</v>
+        <v>0.869015037958476</v>
       </c>
       <c r="H29" s="3">
-        <v>58.41584158415841</v>
+        <v>0.9940594059405941</v>
       </c>
       <c r="I29" s="2">
-        <v>0.07649924658815763</v>
+        <v>0.05971609175986137</v>
       </c>
       <c r="J29" s="3">
-        <v>77.62376237623762</v>
+        <v>0.7148514851485149</v>
       </c>
       <c r="K29" s="3">
-        <v>82.87128712871288</v>
+        <v>0.8282178217821783</v>
       </c>
       <c r="L29" s="4">
-        <v>217</v>
+        <v>627</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1694,37 +1694,37 @@
         <v>40</v>
       </c>
       <c r="B30" s="2">
-        <v>73.25</v>
+        <v>93.81999999999999</v>
       </c>
       <c r="C30" s="2">
-        <v>0.267899164624197</v>
+        <v>1.031225529980981</v>
       </c>
       <c r="D30" s="3">
-        <v>77.02970297029702</v>
+        <v>0.9900990099009901</v>
       </c>
       <c r="E30" s="2">
-        <v>0.4109680211665745</v>
+        <v>0.7121934612097175</v>
       </c>
       <c r="F30" s="3">
-        <v>82.37623762376238</v>
+        <v>0.9643564356435644</v>
       </c>
       <c r="G30" s="2">
-        <v>0.42259020345057</v>
+        <v>0.2267932767367592</v>
       </c>
       <c r="H30" s="3">
-        <v>88.71287128712871</v>
+        <v>0.5821782178217823</v>
       </c>
       <c r="I30" s="2">
-        <v>0.09190273839205082</v>
+        <v>0.07448214173854011</v>
       </c>
       <c r="J30" s="3">
-        <v>82.97029702970298</v>
+        <v>0.7683168316831683</v>
       </c>
       <c r="K30" s="3">
-        <v>82.77227722772277</v>
+        <v>0.8262376237623763</v>
       </c>
       <c r="L30" s="4">
-        <v>273</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1732,37 +1732,37 @@
         <v>41</v>
       </c>
       <c r="B31" s="2">
-        <v>30.87</v>
+        <v>71.84999999999999</v>
       </c>
       <c r="C31" s="2">
-        <v>0.1479868462730729</v>
+        <v>0.265621155765815</v>
       </c>
       <c r="D31" s="3">
-        <v>61.18811881188119</v>
+        <v>0.7663366336633664</v>
       </c>
       <c r="E31" s="2">
-        <v>1.247512157447173</v>
+        <v>0.413629330821879</v>
       </c>
       <c r="F31" s="3">
-        <v>99.60396039603961</v>
+        <v>0.8277227722772277</v>
       </c>
       <c r="G31" s="2">
-        <v>0.8675388410161483</v>
+        <v>0.41257983054182</v>
       </c>
       <c r="H31" s="3">
-        <v>99.4059405940594</v>
+        <v>0.8772277227722772</v>
       </c>
       <c r="I31" s="2">
-        <v>0.05775018736559979</v>
+        <v>0.09180387848538939</v>
       </c>
       <c r="J31" s="3">
-        <v>70.6930693069307</v>
+        <v>0.8297029702970298</v>
       </c>
       <c r="K31" s="3">
-        <v>82.72277227722772</v>
+        <v>0.8252475247524753</v>
       </c>
       <c r="L31" s="4">
-        <v>647</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1770,37 +1770,37 @@
         <v>42</v>
       </c>
       <c r="B32" s="2">
-        <v>304.18</v>
+        <v>301.85</v>
       </c>
       <c r="C32" s="2">
-        <v>0.6698283689318626</v>
+        <v>0.6640735119314289</v>
       </c>
       <c r="D32" s="3">
-        <v>94.85148514851485</v>
+        <v>0.9485148514851486</v>
       </c>
       <c r="E32" s="2">
-        <v>0.2505425467153261</v>
+        <v>0.2528181178344159</v>
       </c>
       <c r="F32" s="3">
-        <v>58.01980198019802</v>
+        <v>0.5861386138613862</v>
       </c>
       <c r="G32" s="2">
-        <v>0.352999390937823</v>
+        <v>0.3616206014376097</v>
       </c>
       <c r="H32" s="3">
-        <v>80.19801980198019</v>
+        <v>0.805940594059406</v>
       </c>
       <c r="I32" s="2">
-        <v>0.1734409491955915</v>
+        <v>0.1707759555187895</v>
       </c>
       <c r="J32" s="3">
-        <v>96.43564356435644</v>
+        <v>0.9603960396039604</v>
       </c>
       <c r="K32" s="3">
-        <v>82.37623762376238</v>
+        <v>0.8252475247524753</v>
       </c>
       <c r="L32" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1808,37 +1808,37 @@
         <v>43</v>
       </c>
       <c r="B33" s="2">
-        <v>25.24</v>
+        <v>24.74</v>
       </c>
       <c r="C33" s="2">
-        <v>0.2103615271755756</v>
+        <v>0.2193013167277825</v>
       </c>
       <c r="D33" s="3">
-        <v>68.71287128712871</v>
+        <v>0.6990099009900991</v>
       </c>
       <c r="E33" s="2">
-        <v>0.439311832109631</v>
+        <v>0.4480860665767503</v>
       </c>
       <c r="F33" s="3">
-        <v>85.14851485148515</v>
+        <v>0.8613861386138614</v>
       </c>
       <c r="G33" s="2">
-        <v>0.3454695041362964</v>
+        <v>0.3334328110724135</v>
       </c>
       <c r="H33" s="3">
-        <v>79.00990099009901</v>
+        <v>0.7683168316831683</v>
       </c>
       <c r="I33" s="2">
-        <v>0.1524161012610642</v>
+        <v>0.1558758347209623</v>
       </c>
       <c r="J33" s="3">
-        <v>93.66336633663366</v>
+        <v>0.9425742574257425</v>
       </c>
       <c r="K33" s="3">
-        <v>81.63366336633663</v>
+        <v>0.8178217821782179</v>
       </c>
       <c r="L33" s="4">
-        <v>792</v>
+        <v>808</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1846,37 +1846,37 @@
         <v>44</v>
       </c>
       <c r="B34" s="2">
-        <v>291.43</v>
+        <v>294.58</v>
       </c>
       <c r="C34" s="2">
-        <v>0.415613725487778</v>
+        <v>0.4050966437278345</v>
       </c>
       <c r="D34" s="3">
-        <v>87.52475247524752</v>
+        <v>0.8633663366336635</v>
       </c>
       <c r="E34" s="2">
-        <v>0.3417713659437648</v>
+        <v>0.3446906095276095</v>
       </c>
       <c r="F34" s="3">
-        <v>73.26732673267327</v>
+        <v>0.7366336633663366</v>
       </c>
       <c r="G34" s="2">
-        <v>0.4491486485811158</v>
+        <v>0.4563577888400481</v>
       </c>
       <c r="H34" s="3">
-        <v>90.0990099009901</v>
+        <v>0.900990099009901</v>
       </c>
       <c r="I34" s="2">
-        <v>0.07030439404881822</v>
+        <v>0.06975969618408126</v>
       </c>
       <c r="J34" s="3">
-        <v>75.04950495049505</v>
+        <v>0.7465346534653466</v>
       </c>
       <c r="K34" s="3">
-        <v>81.48514851485149</v>
+        <v>0.8118811881188119</v>
       </c>
       <c r="L34" s="4">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1884,37 +1884,37 @@
         <v>45</v>
       </c>
       <c r="B35" s="2">
-        <v>39.9</v>
+        <v>40.7</v>
       </c>
       <c r="C35" s="2">
-        <v>0.3955321807760373</v>
+        <v>0.4127478293083173</v>
       </c>
       <c r="D35" s="3">
-        <v>85.74257425742574</v>
+        <v>0.8732673267326733</v>
       </c>
       <c r="E35" s="2">
-        <v>0.4563029042522723</v>
+        <v>0.4602777525589518</v>
       </c>
       <c r="F35" s="3">
-        <v>86.93069306930693</v>
+        <v>0.8693069306930693</v>
       </c>
       <c r="G35" s="2">
-        <v>0.4454949297379418</v>
+        <v>0.441094468889126</v>
       </c>
       <c r="H35" s="3">
-        <v>89.9009900990099</v>
+        <v>0.897029702970297</v>
       </c>
       <c r="I35" s="2">
-        <v>0.03850159227308345</v>
+        <v>0.03700506741568101</v>
       </c>
       <c r="J35" s="3">
-        <v>60.3960396039604</v>
+        <v>0.5980198019801981</v>
       </c>
       <c r="K35" s="3">
-        <v>80.74257425742574</v>
+        <v>0.8094059405940595</v>
       </c>
       <c r="L35" s="4">
-        <v>501</v>
+        <v>491</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1922,37 +1922,37 @@
         <v>46</v>
       </c>
       <c r="B36" s="2">
-        <v>86.43000000000001</v>
+        <v>85.93000000000001</v>
       </c>
       <c r="C36" s="2">
-        <v>0.4111603233882284</v>
+        <v>0.4072656874098877</v>
       </c>
       <c r="D36" s="3">
-        <v>87.12871287128714</v>
+        <v>0.8693069306930693</v>
       </c>
       <c r="E36" s="2">
-        <v>0.3942900894336595</v>
+        <v>0.4000144756868177</v>
       </c>
       <c r="F36" s="3">
-        <v>80</v>
+        <v>0.807920792079208</v>
       </c>
       <c r="G36" s="2">
-        <v>0.4816183678830325</v>
+        <v>0.478950023183581</v>
       </c>
       <c r="H36" s="3">
-        <v>92.07920792079207</v>
+        <v>0.9227722772277228</v>
       </c>
       <c r="I36" s="2">
-        <v>0.04543032113975107</v>
+        <v>0.0454618050987854</v>
       </c>
       <c r="J36" s="3">
-        <v>63.56435643564357</v>
+        <v>0.6356435643564357</v>
       </c>
       <c r="K36" s="3">
-        <v>80.6930693069307</v>
+        <v>0.808910891089109</v>
       </c>
       <c r="L36" s="4">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1960,37 +1960,37 @@
         <v>47</v>
       </c>
       <c r="B37" s="2">
-        <v>152.67</v>
+        <v>149.43</v>
       </c>
       <c r="C37" s="2">
-        <v>0.7360122255985719</v>
+        <v>0.7188976104985362</v>
       </c>
       <c r="D37" s="3">
-        <v>95.84158415841584</v>
+        <v>0.9564356435643565</v>
       </c>
       <c r="E37" s="2">
-        <v>0.6905838057194331</v>
+        <v>0.6913515756520913</v>
       </c>
       <c r="F37" s="3">
-        <v>96.03960396039604</v>
+        <v>0.9584158415841584</v>
       </c>
       <c r="G37" s="2">
-        <v>0.3435300044334814</v>
+        <v>0.3406146936441806</v>
       </c>
       <c r="H37" s="3">
-        <v>78.01980198019803</v>
+        <v>0.7801980198019802</v>
       </c>
       <c r="I37" s="2">
-        <v>0.02721367224701757</v>
+        <v>0.02681534047139606</v>
       </c>
       <c r="J37" s="3">
-        <v>52.07920792079208</v>
+        <v>0.5188118811881188</v>
       </c>
       <c r="K37" s="3">
-        <v>80.4950495049505</v>
+        <v>0.8034653465346535</v>
       </c>
       <c r="L37" s="4">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1998,37 +1998,37 @@
         <v>48</v>
       </c>
       <c r="B38" s="2">
-        <v>54.33</v>
+        <v>86.94</v>
       </c>
       <c r="C38" s="2">
-        <v>0.09846606355238317</v>
+        <v>0.4366524504975828</v>
       </c>
       <c r="D38" s="3">
-        <v>53.46534653465346</v>
+        <v>0.8930693069306931</v>
       </c>
       <c r="E38" s="2">
-        <v>0.4791277207573937</v>
+        <v>0.4205288468408785</v>
       </c>
       <c r="F38" s="3">
-        <v>89.5049504950495</v>
+        <v>0.8415841584158416</v>
       </c>
       <c r="G38" s="2">
-        <v>0.5298666723643934</v>
+        <v>0.337176677610979</v>
       </c>
       <c r="H38" s="3">
-        <v>94.45544554455445</v>
+        <v>0.7742574257425743</v>
       </c>
       <c r="I38" s="2">
-        <v>0.08705230177141451</v>
+        <v>0.0508058240976281</v>
       </c>
       <c r="J38" s="3">
-        <v>81.58415841584159</v>
+        <v>0.6732673267326733</v>
       </c>
       <c r="K38" s="3">
-        <v>79.75247524752476</v>
+        <v>0.7955445544554456</v>
       </c>
       <c r="L38" s="4">
-        <v>368</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -2036,37 +2036,37 @@
         <v>49</v>
       </c>
       <c r="B39" s="2">
-        <v>176.26</v>
+        <v>52.5</v>
       </c>
       <c r="C39" s="2">
-        <v>0.2664146519515195</v>
+        <v>0.09449497596953119</v>
       </c>
       <c r="D39" s="3">
-        <v>76.83168316831683</v>
+        <v>0.5287128712871287</v>
       </c>
       <c r="E39" s="2">
-        <v>0.2931666932016621</v>
+        <v>0.4753886343736136</v>
       </c>
       <c r="F39" s="3">
-        <v>66.53465346534654</v>
+        <v>0.887128712871287</v>
       </c>
       <c r="G39" s="2">
-        <v>0.4990156875253701</v>
+        <v>0.525252005785713</v>
       </c>
       <c r="H39" s="3">
-        <v>92.87128712871286</v>
+        <v>0.9405940594059407</v>
       </c>
       <c r="I39" s="2">
-        <v>0.0849468387902457</v>
+        <v>0.08900305896132638</v>
       </c>
       <c r="J39" s="3">
-        <v>80.79207920792079</v>
+        <v>0.8198019801980198</v>
       </c>
       <c r="K39" s="3">
-        <v>79.25742574257426</v>
+        <v>0.7940594059405941</v>
       </c>
       <c r="L39" s="4">
-        <v>113</v>
+        <v>380</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -2074,37 +2074,37 @@
         <v>50</v>
       </c>
       <c r="B40" s="2">
-        <v>87.8</v>
+        <v>180.28</v>
       </c>
       <c r="C40" s="2">
-        <v>0.444427367001473</v>
+        <v>0.2667628485482316</v>
       </c>
       <c r="D40" s="3">
-        <v>90.0990099009901</v>
+        <v>0.7702970297029702</v>
       </c>
       <c r="E40" s="2">
-        <v>0.4050755256929217</v>
+        <v>0.2900119583825087</v>
       </c>
       <c r="F40" s="3">
-        <v>81.38613861386139</v>
+        <v>0.6594059405940594</v>
       </c>
       <c r="G40" s="2">
-        <v>0.339843020176303</v>
+        <v>0.494463002454601</v>
       </c>
       <c r="H40" s="3">
-        <v>77.82178217821782</v>
+        <v>0.9267326732673267</v>
       </c>
       <c r="I40" s="2">
-        <v>0.0505786393498805</v>
+        <v>0.0851022348347102</v>
       </c>
       <c r="J40" s="3">
-        <v>67.52475247524752</v>
+        <v>0.8099009900990098</v>
       </c>
       <c r="K40" s="3">
-        <v>79.20792079207921</v>
+        <v>0.7915841584158415</v>
       </c>
       <c r="L40" s="4">
-        <v>227</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2112,37 +2112,37 @@
         <v>51</v>
       </c>
       <c r="B41" s="2">
-        <v>440.73</v>
+        <v>95.06</v>
       </c>
       <c r="C41" s="2">
-        <v>0.3973377546319791</v>
+        <v>-0.09808929076991034</v>
       </c>
       <c r="D41" s="3">
-        <v>86.13861386138613</v>
+        <v>0.2514851485148515</v>
       </c>
       <c r="E41" s="2">
-        <v>0.4030306094802433</v>
+        <v>0.9650102033274236</v>
       </c>
       <c r="F41" s="3">
-        <v>81.18811881188118</v>
+        <v>0.9881188118811882</v>
       </c>
       <c r="G41" s="2">
-        <v>0.22853132602925</v>
+        <v>0.5460854558994732</v>
       </c>
       <c r="H41" s="3">
-        <v>58.81188118811881</v>
+        <v>0.9504950495049505</v>
       </c>
       <c r="I41" s="2">
-        <v>0.113088091653903</v>
+        <v>0.1673215244620989</v>
       </c>
       <c r="J41" s="3">
-        <v>88.71287128712871</v>
+        <v>0.9564356435643565</v>
       </c>
       <c r="K41" s="3">
-        <v>78.71287128712871</v>
+        <v>0.7866336633663367</v>
       </c>
       <c r="L41" s="4">
-        <v>45</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2150,37 +2150,37 @@
         <v>52</v>
       </c>
       <c r="B42" s="2">
-        <v>233.04</v>
+        <v>122.74</v>
       </c>
       <c r="C42" s="2">
-        <v>0.37819897679906</v>
+        <v>0.1161495775786699</v>
       </c>
       <c r="D42" s="3">
-        <v>84.55445544554455</v>
+        <v>0.5663366336633664</v>
       </c>
       <c r="E42" s="2">
-        <v>0.5146950450488615</v>
+        <v>0.6007531165534129</v>
       </c>
       <c r="F42" s="3">
-        <v>92.07920792079207</v>
+        <v>0.9445544554455445</v>
       </c>
       <c r="G42" s="2">
-        <v>0.4453749734144927</v>
+        <v>0.3474131606364216</v>
       </c>
       <c r="H42" s="3">
-        <v>89.70297029702971</v>
+        <v>0.7920792079207921</v>
       </c>
       <c r="I42" s="2">
-        <v>0.02093905892979452</v>
+        <v>0.09345793382416828</v>
       </c>
       <c r="J42" s="3">
-        <v>48.31683168316832</v>
+        <v>0.8356435643564356</v>
       </c>
       <c r="K42" s="3">
-        <v>78.66336633663366</v>
+        <v>0.7846534653465347</v>
       </c>
       <c r="L42" s="4">
-        <v>85</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2188,37 +2188,37 @@
         <v>53</v>
       </c>
       <c r="B43" s="2">
-        <v>20.33</v>
+        <v>847</v>
       </c>
       <c r="C43" s="2">
-        <v>0.01855386136991235</v>
+        <v>0.3557408588246135</v>
       </c>
       <c r="D43" s="3">
-        <v>42.17821782178218</v>
+        <v>0.8277227722772277</v>
       </c>
       <c r="E43" s="2">
-        <v>0.3895363450245142</v>
+        <v>0.3940981957783558</v>
       </c>
       <c r="F43" s="3">
-        <v>79.60396039603961</v>
+        <v>0.8</v>
       </c>
       <c r="G43" s="2">
-        <v>0.4997920393695846</v>
+        <v>0.2391655589506806</v>
       </c>
       <c r="H43" s="3">
-        <v>93.06930693069307</v>
+        <v>0.6039603960396039</v>
       </c>
       <c r="I43" s="2">
-        <v>0.2541129393042452</v>
+        <v>0.1278094105792779</v>
       </c>
       <c r="J43" s="3">
-        <v>99.4059405940594</v>
+        <v>0.904950495049505</v>
       </c>
       <c r="K43" s="3">
-        <v>78.56435643564356</v>
+        <v>0.7841584158415842</v>
       </c>
       <c r="L43" s="4">
-        <v>983</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -2226,37 +2226,37 @@
         <v>54</v>
       </c>
       <c r="B44" s="2">
-        <v>94.8</v>
+        <v>21.22</v>
       </c>
       <c r="C44" s="2">
-        <v>-0.1001781626553349</v>
+        <v>0.01848050138469962</v>
       </c>
       <c r="D44" s="3">
-        <v>24.55445544554455</v>
+        <v>0.4217821782178218</v>
       </c>
       <c r="E44" s="2">
-        <v>0.9662175612121283</v>
+        <v>0.3806064918913287</v>
       </c>
       <c r="F44" s="3">
-        <v>98.81188118811882</v>
+        <v>0.7821782178217822</v>
       </c>
       <c r="G44" s="2">
-        <v>0.5276035113337805</v>
+        <v>0.5108338108254566</v>
       </c>
       <c r="H44" s="3">
-        <v>94.25742574257426</v>
+        <v>0.9386138613861387</v>
       </c>
       <c r="I44" s="2">
-        <v>0.1699881716503722</v>
+        <v>0.257822732173318</v>
       </c>
       <c r="J44" s="3">
-        <v>95.84158415841584</v>
+        <v>0.9940594059405941</v>
       </c>
       <c r="K44" s="3">
-        <v>78.36633663366337</v>
+        <v>0.7841584158415842</v>
       </c>
       <c r="L44" s="4">
-        <v>210</v>
+        <v>942</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2264,37 +2264,37 @@
         <v>55</v>
       </c>
       <c r="B45" s="2">
-        <v>18.07</v>
+        <v>35.22</v>
       </c>
       <c r="C45" s="2">
-        <v>0.02736945683621016</v>
+        <v>0.135411184219742</v>
       </c>
       <c r="D45" s="3">
-        <v>43.16831683168317</v>
+        <v>0.5980198019801981</v>
       </c>
       <c r="E45" s="2">
-        <v>0.6003639558619575</v>
+        <v>0.4933852283373146</v>
       </c>
       <c r="F45" s="3">
-        <v>93.66336633663366</v>
+        <v>0.904950495049505</v>
       </c>
       <c r="G45" s="2">
-        <v>0.7096229774342088</v>
+        <v>0.265949113036722</v>
       </c>
       <c r="H45" s="3">
-        <v>98.01980198019803</v>
+        <v>0.6673267326732674</v>
       </c>
       <c r="I45" s="2">
-        <v>0.07737911546787962</v>
+        <v>0.1680619425882676</v>
       </c>
       <c r="J45" s="3">
-        <v>78.01980198019803</v>
+        <v>0.9584158415841584</v>
       </c>
       <c r="K45" s="3">
-        <v>78.21782178217822</v>
+        <v>0.7821782178217822</v>
       </c>
       <c r="L45" s="4">
-        <v>1106</v>
+        <v>567</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2302,37 +2302,37 @@
         <v>56</v>
       </c>
       <c r="B46" s="2">
-        <v>123.32</v>
+        <v>18.2</v>
       </c>
       <c r="C46" s="2">
-        <v>0.1139452842482498</v>
+        <v>0.02646802193691759</v>
       </c>
       <c r="D46" s="3">
-        <v>56.43564356435643</v>
+        <v>0.4316831683168317</v>
       </c>
       <c r="E46" s="2">
-        <v>0.6161392106236063</v>
+        <v>0.592507919979709</v>
       </c>
       <c r="F46" s="3">
-        <v>94.25742574257426</v>
+        <v>0.9366336633663366</v>
       </c>
       <c r="G46" s="2">
-        <v>0.3437404361459169</v>
+        <v>0.7081511611693845</v>
       </c>
       <c r="H46" s="3">
-        <v>78.61386138613861</v>
+        <v>0.9821782178217822</v>
       </c>
       <c r="I46" s="2">
-        <v>0.0925519624520145</v>
+        <v>0.07649307203014698</v>
       </c>
       <c r="J46" s="3">
-        <v>83.36633663366337</v>
+        <v>0.7762376237623763</v>
       </c>
       <c r="K46" s="3">
-        <v>78.16831683168317</v>
+        <v>0.7816831683168317</v>
       </c>
       <c r="L46" s="4">
-        <v>162</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2340,37 +2340,37 @@
         <v>57</v>
       </c>
       <c r="B47" s="2">
-        <v>28.53</v>
+        <v>239.68</v>
       </c>
       <c r="C47" s="2">
-        <v>-0.1213151565780334</v>
+        <v>0.3687605910990718</v>
       </c>
       <c r="D47" s="3">
-        <v>22.97029702970297</v>
+        <v>0.8376237623762377</v>
       </c>
       <c r="E47" s="2">
-        <v>0.8704686948518691</v>
+        <v>0.5026444308657819</v>
       </c>
       <c r="F47" s="3">
-        <v>98.61386138613861</v>
+        <v>0.9108910891089108</v>
       </c>
       <c r="G47" s="2">
-        <v>0.7122731212638974</v>
+        <v>0.4272857264311102</v>
       </c>
       <c r="H47" s="3">
-        <v>98.21782178217822</v>
+        <v>0.8891089108910891</v>
       </c>
       <c r="I47" s="2">
-        <v>0.1459938708332565</v>
+        <v>0.02142672158372082</v>
       </c>
       <c r="J47" s="3">
-        <v>92.67326732673267</v>
+        <v>0.4851485148514851</v>
       </c>
       <c r="K47" s="3">
-        <v>78.11881188118812</v>
+        <v>0.7806930693069307</v>
       </c>
       <c r="L47" s="4">
-        <v>701</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -2378,37 +2378,37 @@
         <v>58</v>
       </c>
       <c r="B48" s="2">
-        <v>31.03</v>
+        <v>32.15</v>
       </c>
       <c r="C48" s="2">
-        <v>-0.06984150551416959</v>
+        <v>-0.0702441402986879</v>
       </c>
       <c r="D48" s="3">
-        <v>28.11881188118812</v>
+        <v>0.2792079207920792</v>
       </c>
       <c r="E48" s="2">
-        <v>0.6911893136729524</v>
+        <v>0.70185474743597</v>
       </c>
       <c r="F48" s="3">
-        <v>96.23762376237623</v>
+        <v>0.9603960396039604</v>
       </c>
       <c r="G48" s="2">
-        <v>0.4576254282519833</v>
+        <v>0.4647953604340588</v>
       </c>
       <c r="H48" s="3">
-        <v>90.4950495049505</v>
+        <v>0.9089108910891089</v>
       </c>
       <c r="I48" s="2">
-        <v>0.1905549655327469</v>
+        <v>0.18815591263521</v>
       </c>
       <c r="J48" s="3">
-        <v>97.22772277227723</v>
+        <v>0.9722772277227724</v>
       </c>
       <c r="K48" s="3">
-        <v>78.01980198019803</v>
+        <v>0.7801980198019802</v>
       </c>
       <c r="L48" s="4">
-        <v>644</v>
+        <v>622</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -2416,37 +2416,37 @@
         <v>59</v>
       </c>
       <c r="B49" s="2">
-        <v>39.04</v>
+        <v>447.23</v>
       </c>
       <c r="C49" s="2">
-        <v>-0.1954095100522804</v>
+        <v>0.3993511124816974</v>
       </c>
       <c r="D49" s="3">
-        <v>13.66336633663366</v>
+        <v>0.8574257425742574</v>
       </c>
       <c r="E49" s="2">
-        <v>0.8405337260257675</v>
+        <v>0.3979739756564899</v>
       </c>
       <c r="F49" s="3">
-        <v>98.41584158415841</v>
+        <v>0.805940594059406</v>
       </c>
       <c r="G49" s="2">
-        <v>0.980537442864041</v>
+        <v>0.2235846344445158</v>
       </c>
       <c r="H49" s="3">
-        <v>99.80198019801981</v>
+        <v>0.5722772277227722</v>
       </c>
       <c r="I49" s="2">
-        <v>0.2943625006340714</v>
+        <v>0.1133810778774512</v>
       </c>
       <c r="J49" s="3">
-        <v>100</v>
+        <v>0.8851485148514852</v>
       </c>
       <c r="K49" s="3">
-        <v>77.97029702970298</v>
+        <v>0.7801980198019802</v>
       </c>
       <c r="L49" s="4">
-        <v>512</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2454,37 +2454,37 @@
         <v>60</v>
       </c>
       <c r="B50" s="2">
-        <v>35.52</v>
+        <v>39.14</v>
       </c>
       <c r="C50" s="2">
-        <v>0.1387318497274285</v>
+        <v>-0.1933324774156136</v>
       </c>
       <c r="D50" s="3">
-        <v>59.80198019801981</v>
+        <v>0.1366336633663366</v>
       </c>
       <c r="E50" s="2">
-        <v>0.5043235535974985</v>
+        <v>0.8327517858978472</v>
       </c>
       <c r="F50" s="3">
-        <v>91.08910891089108</v>
+        <v>0.9841584158415841</v>
       </c>
       <c r="G50" s="2">
-        <v>0.260053891831938</v>
+        <v>0.9778393249484451</v>
       </c>
       <c r="H50" s="3">
-        <v>65.74257425742574</v>
+        <v>0.998019801980198</v>
       </c>
       <c r="I50" s="2">
-        <v>0.1618726943993328</v>
+        <v>0.2940074493537081</v>
       </c>
       <c r="J50" s="3">
-        <v>95.04950495049505</v>
+        <v>1</v>
       </c>
       <c r="K50" s="3">
-        <v>77.92079207920793</v>
+        <v>0.7797029702970297</v>
       </c>
       <c r="L50" s="4">
-        <v>563</v>
+        <v>510</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2492,37 +2492,37 @@
         <v>61</v>
       </c>
       <c r="B51" s="2">
-        <v>834</v>
+        <v>27.44</v>
       </c>
       <c r="C51" s="2">
-        <v>0.3680704377328896</v>
+        <v>-0.1197412206023989</v>
       </c>
       <c r="D51" s="3">
-        <v>83.36633663366337</v>
+        <v>0.2297029702970297</v>
       </c>
       <c r="E51" s="2">
-        <v>0.3767832555937105</v>
+        <v>0.8817368294627661</v>
       </c>
       <c r="F51" s="3">
-        <v>77.42574257425743</v>
+        <v>0.9861386138613861</v>
       </c>
       <c r="G51" s="2">
-        <v>0.2350209617919372</v>
+        <v>0.6950202256479153</v>
       </c>
       <c r="H51" s="3">
-        <v>60</v>
+        <v>0.9782178217821782</v>
       </c>
       <c r="I51" s="2">
-        <v>0.1269703734467672</v>
+        <v>0.1426180428200647</v>
       </c>
       <c r="J51" s="3">
-        <v>90.6930693069307</v>
+        <v>0.9227722772277228</v>
       </c>
       <c r="K51" s="3">
-        <v>77.87128712871288</v>
+        <v>0.7792079207920792</v>
       </c>
       <c r="L51" s="4">
-        <v>23</v>
+        <v>728</v>
       </c>
     </row>
   </sheetData>

</xml_diff>